<commit_message>
modify to be BaseCase
</commit_message>
<xml_diff>
--- a/Granule/AOBNOBAMX.xlsx
+++ b/Granule/AOBNOBAMX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2424069M\Desktop\UofG\PhD\0. AOB&amp;NOB sim\SIM\Granule\0. AOBNOBAMX\BaseCase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Uni\Master Thesis\version_GitHub\Granule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840B8B20-0E3D-4B84-8A68-7A22F99D55DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B866FD19-3034-4540-9A57-1EC0F70496D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reactions" sheetId="18" r:id="rId1"/>
@@ -25,17 +25,12 @@
     <sheet name="Diffusion" sheetId="28" r:id="rId10"/>
     <sheet name="Tolerances" sheetId="29" r:id="rId11"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId12"/>
-  </externalReferences>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -56,52 +51,88 @@
   <commentList>
     <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     AOB and NOB: calculated [Rebeca]</t>
+        </r>
       </text>
     </comment>
     <comment ref="F2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     FNA (HNO2) [Jubany2008]</t>
+        </r>
       </text>
     </comment>
     <comment ref="E3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     FA (NH3) [Kim2008, Blackburne2007a]</t>
+        </r>
       </text>
     </comment>
     <comment ref="E4" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     FA (NH3) [Kim2008, Blackburne2007a]</t>
+        </r>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     From [Straka2019]
 Reply:
     Assume NH3 and HNO2 uptake</t>
+        </r>
       </text>
     </comment>
     <comment ref="H5" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     From [Strous1998]</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -3039,45 +3070,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Reactions"/>
-      <sheetName val="SpecParam"/>
-      <sheetName val="ReactionMatrix"/>
-      <sheetName val="States"/>
-      <sheetName val="Influent"/>
-      <sheetName val="ThermoParam"/>
-      <sheetName val="Bacteria"/>
-      <sheetName val="Parameters"/>
-      <sheetName val="Discretization"/>
-      <sheetName val="Diffusion"/>
-      <sheetName val="Tolerances"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6">
-        <row r="6">
-          <cell r="B6">
-            <v>1E-3</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Eloi Martínez-Rabert (PGR)" id="{5CC223E8-22CF-48C3-ABCE-0A00391E726E}" userId="S::2424069M@student.gla.ac.uk::cb616271-4a7a-48f5-8972-853218eda004" providerId="AD"/>
@@ -3431,7 +3423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="B2:AN39"/>
@@ -5988,6 +5980,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6097,6 +6090,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6200,10 +6194,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6445,6 +6440,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7343,6 +7339,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7581,10 +7578,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7660,8 +7658,8 @@
         <v>89</v>
       </c>
       <c r="B4" s="181">
-        <f>(1)/(32*1000)</f>
-        <v>3.1250000000000001E-5</v>
+        <f>(6)/(32*1000)</f>
+        <v>1.875E-4</v>
       </c>
       <c r="C4" s="176" t="s">
         <v>95</v>
@@ -7770,6 +7768,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8546,6 +8545,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8737,10 +8737,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8909,10 +8910,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8926,8 +8928,7 @@
         <v>130</v>
       </c>
       <c r="B1" s="227">
-        <f>B3/B5</f>
-        <v>255.00000000000003</v>
+        <v>257</v>
       </c>
       <c r="C1" s="155" t="s">
         <v>114</v>
@@ -8940,8 +8941,7 @@
         <v>131</v>
       </c>
       <c r="B2" s="228">
-        <f>B4/B6</f>
-        <v>255.00000000000003</v>
+        <v>257</v>
       </c>
       <c r="C2" s="157" t="s">
         <v>114</v>
@@ -8954,8 +8954,8 @@
         <v>132</v>
       </c>
       <c r="B3" s="229">
-        <f>([1]Bacteria!B6+2*B8+10*10^(-6))</f>
-        <v>1.0200000000000001E-3</v>
+        <f>B1*B5</f>
+        <v>1.0280000000000001E-3</v>
       </c>
       <c r="C3" s="157" t="s">
         <v>106</v>
@@ -8968,8 +8968,8 @@
         <v>133</v>
       </c>
       <c r="B4" s="229">
-        <f>([1]Bacteria!B6+2*B8+10*10^(-6))</f>
-        <v>1.0200000000000001E-3</v>
+        <f>B2*B6</f>
+        <v>1.0280000000000001E-3</v>
       </c>
       <c r="C4" s="157" t="s">
         <v>106</v>
@@ -9038,8 +9038,8 @@
         <v>138</v>
       </c>
       <c r="B9" s="230">
-        <f>400*24</f>
-        <v>9600</v>
+        <f>100*24</f>
+        <v>2400</v>
       </c>
       <c r="C9" s="157" t="s">
         <v>127</v>
@@ -9052,7 +9052,7 @@
         <v>139</v>
       </c>
       <c r="B10" s="229">
-        <v>9.9999999999999995E-7</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="C10" s="157" t="s">
         <v>127</v>
@@ -9091,8 +9091,8 @@
         <v>142</v>
       </c>
       <c r="B13" s="231">
-        <f>4*24</f>
-        <v>96</v>
+        <f>1*24</f>
+        <v>24</v>
       </c>
       <c r="C13" s="172" t="s">
         <v>127</v>

</xml_diff>